<commit_message>
update gaussian copula ;
</commit_message>
<xml_diff>
--- a/simulation_study4/simParamsSummary.xlsx
+++ b/simulation_study4/simParamsSummary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caitl\Documents\Postdoc\multipleDataBCM\simulation_study2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caitl\Documents\Postdoc\multipleDataBCM\simulation_study4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1517128B-8688-4FB7-B4A6-98B866DA9F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614C3588-47BF-4884-B7A0-596F86038622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24576" yWindow="-2712" windowWidth="17280" windowHeight="8880" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{172EBA67-DF58-4CEE-BF06-48D6A2384BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,22 +88,22 @@
     <t>x0C</t>
   </si>
   <si>
+    <t>nuD</t>
+  </si>
+  <si>
+    <t>x0D</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
     <t>deltaC</t>
   </si>
   <si>
     <t>deltaD</t>
-  </si>
-  <si>
-    <t>nuD</t>
-  </si>
-  <si>
-    <t>x0D</t>
-  </si>
-  <si>
-    <t>death</t>
-  </si>
-  <si>
-    <t>equal</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +514,7 @@
         <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>15</v>
@@ -523,13 +523,13 @@
         <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>0.85</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>0.85</v>

</xml_diff>